<commit_message>
se subio la informacion del fin de semana
</commit_message>
<xml_diff>
--- a/2015-2016/clases/informatica_basica/a/evaluacion.xlsx
+++ b/2015-2016/clases/informatica_basica/a/evaluacion.xlsx
@@ -156,6 +156,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -178,6 +179,7 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -185,6 +187,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -192,11 +195,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -282,7 +287,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -376,9 +381,11 @@
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="N7" s="5" t="e">
+      <c r="N7" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D7:M7)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -388,9 +395,11 @@
       <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N8" s="5" t="e">
+      <c r="N8" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D8:M8)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -400,9 +409,11 @@
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N9" s="5" t="e">
+      <c r="N9" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D9:M9)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -412,9 +423,11 @@
       <c r="C10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N10" s="5" t="e">
+      <c r="N10" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D10:M10)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -424,9 +437,11 @@
       <c r="C11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N11" s="5" t="e">
+      <c r="N11" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D11:M11)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -436,9 +451,11 @@
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="N12" s="5" t="e">
+      <c r="N12" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D12:M12)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -448,9 +465,11 @@
       <c r="C13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N13" s="5" t="e">
+      <c r="N13" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D13:M13)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -460,9 +479,11 @@
       <c r="C14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N14" s="5" t="e">
+      <c r="N14" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D14:M14)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -472,9 +493,11 @@
       <c r="C15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N15" s="5" t="e">
+      <c r="N15" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D15:M15)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -484,9 +507,11 @@
       <c r="C16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N16" s="5" t="e">
+      <c r="N16" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D16:M16)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -496,9 +521,11 @@
       <c r="C17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N17" s="5" t="e">
+      <c r="N17" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D17:M17)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -508,9 +535,11 @@
       <c r="C18" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="N18" s="5" t="e">
+      <c r="N18" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D18:M18)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -520,9 +549,11 @@
       <c r="C19" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N19" s="5" t="e">
+      <c r="N19" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D19:M19)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -532,9 +563,11 @@
       <c r="C20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="N20" s="5" t="e">
+      <c r="N20" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D20:M20)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -544,9 +577,11 @@
       <c r="C21" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N21" s="5" t="e">
+      <c r="N21" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D21:M21)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -556,9 +591,11 @@
       <c r="C22" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N22" s="5" t="e">
+      <c r="N22" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D22:M22)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -568,9 +605,11 @@
       <c r="C23" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N23" s="5" t="e">
+      <c r="N23" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D23:M23)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -580,9 +619,11 @@
       <c r="C24" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="N24" s="5" t="e">
+      <c r="N24" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D24:M24)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -592,9 +633,11 @@
       <c r="C25" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="N25" s="5" t="e">
+      <c r="N25" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D25:M25)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -604,9 +647,11 @@
       <c r="C26" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N26" s="5" t="e">
+      <c r="N26" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D26:M26)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -616,9 +661,11 @@
       <c r="C27" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="N27" s="5" t="e">
+      <c r="N27" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D27:M27)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -628,9 +675,11 @@
       <c r="C28" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N28" s="5" t="e">
+      <c r="N28" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D28:M28)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -640,9 +689,11 @@
       <c r="C29" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="N29" s="5" t="e">
+      <c r="N29" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D29:M29)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -652,9 +703,11 @@
       <c r="C30" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="N30" s="5" t="e">
+      <c r="N30" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D30:M30)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -664,9 +717,11 @@
       <c r="C31" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N31" s="5" t="e">
+      <c r="N31" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D31:M31)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -676,9 +731,11 @@
       <c r="C32" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="N32" s="5" t="e">
+      <c r="N32" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D32:M32)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -688,9 +745,11 @@
       <c r="C33" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="N33" s="5" t="e">
+      <c r="N33" s="5" t="inlineStr">
         <f aca="false">AVERAGE(D33:M33)*15/10</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -746,8 +805,8 @@
   </sheetPr>
   <dimension ref="C5:H38"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -822,7 +881,7 @@
         <v>6</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -833,7 +892,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -854,6 +913,9 @@
       <c r="D13" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="E13" s="0" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="n">
@@ -928,6 +990,9 @@
       <c r="D20" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="E20" s="0" t="n">
+        <v>85</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="n">
@@ -969,6 +1034,9 @@
       <c r="D24" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="E24" s="0" t="n">
+        <v>90</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="0" t="n">
@@ -999,6 +1067,9 @@
       <c r="D27" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="E27" s="0" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="0" t="n">
@@ -1051,6 +1122,9 @@
       <c r="D32" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="E32" s="0" t="n">
+        <v>55</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="0" t="n">
@@ -1070,6 +1144,9 @@
       <c r="D34" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="E34" s="0" t="n">
+        <v>80</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="0" t="n">
@@ -1078,6 +1155,9 @@
       <c r="D35" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="E35" s="0" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="0" t="n">
@@ -1085,6 +1165,9 @@
       </c>
       <c r="D36" s="4" t="s">
         <v>32</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>